<commit_message>
Create Markes & Certificate file
</commit_message>
<xml_diff>
--- a/resources/views/resources/database/TSP Management.xlsx
+++ b/resources/views/resources/database/TSP Management.xlsx
@@ -24,41 +24,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>HP</author>
-  </authors>
-  <commentList>
-    <comment ref="D10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>HP:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Ai description ta ki amara aikhan theke add korbo naki course category theke asbe?
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="99">
   <si>
@@ -363,7 +328,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,28 +383,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="3" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,12 +424,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,6 +503,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -573,8 +513,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,15 +825,15 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
@@ -912,13 +851,13 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -1256,11 +1195,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,26 +1217,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
@@ -1602,12 +1541,12 @@
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="5"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
@@ -1617,6 +1556,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>